<commit_message>
updated final time rounded
</commit_message>
<xml_diff>
--- a/Final Results/Data/2.1-Final-data-for-graphs (1).xlsx
+++ b/Final Results/Data/2.1-Final-data-for-graphs (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Data\Desktop\Final Major Project\Results\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Data\Desktop\Final Results\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7274F950-74A8-4AB6-A03C-4B7ABBEFA011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DC7717-9CEC-49D7-856F-36D0BE00AE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7BD4C793-AC5F-4493-AE42-684147676CA2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Excluding Timeout</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Time(m)</t>
+  </si>
+  <si>
+    <t>Number of Requests(Rounded)</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,6 +316,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -631,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2831FB06-038D-4A17-A6D0-D8FABB55FC15}">
   <dimension ref="B2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +647,8 @@
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1224,6 +1231,9 @@
         <v>32</v>
       </c>
       <c r="G36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1231,7 +1241,7 @@
       <c r="C37" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="17">
         <f>727.4/60</f>
         <v>12.123333333333333</v>
@@ -1239,7 +1249,10 @@
       <c r="F37" s="12">
         <v>727.4</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="19">
+        <v>99.6</v>
+      </c>
+      <c r="H37" s="12">
         <v>99.6</v>
       </c>
     </row>
@@ -1247,7 +1260,7 @@
       <c r="C38" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="17">
         <f>891.2/60</f>
         <v>14.853333333333333</v>
@@ -1255,7 +1268,10 @@
       <c r="F38" s="12">
         <v>891.2</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="19">
+        <v>105.6</v>
+      </c>
+      <c r="H38" s="12">
         <v>105.6</v>
       </c>
     </row>
@@ -1263,7 +1279,7 @@
       <c r="C39" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="12"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="17">
         <f>981.1/60</f>
         <v>16.351666666666667</v>
@@ -1271,7 +1287,10 @@
       <c r="F39" s="12">
         <v>981.1</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="19">
+        <v>106.1</v>
+      </c>
+      <c r="H39" s="12">
         <v>106.1</v>
       </c>
     </row>
@@ -1279,7 +1298,7 @@
       <c r="C40" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="12"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="17">
         <f>1252/60</f>
         <v>20.866666666666667</v>
@@ -1287,7 +1306,10 @@
       <c r="F40" s="12">
         <v>1251.7</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="19">
+        <v>116.3</v>
+      </c>
+      <c r="H40" s="12">
         <v>116.3</v>
       </c>
     </row>
@@ -1295,7 +1317,7 @@
       <c r="C41" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="17">
         <f>1289/60</f>
         <v>21.483333333333334</v>
@@ -1303,7 +1325,10 @@
       <c r="F41" s="12">
         <v>1289.3</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="19">
+        <v>120</v>
+      </c>
+      <c r="H41" s="12">
         <v>120</v>
       </c>
     </row>
@@ -1311,7 +1336,7 @@
       <c r="C42" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="12"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="17">
         <f>919.9/60</f>
         <v>15.331666666666667</v>
@@ -1319,7 +1344,10 @@
       <c r="F42" s="12">
         <v>919.9</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="19">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="H42" s="12">
         <v>128.69999999999999</v>
       </c>
     </row>
@@ -1327,7 +1355,7 @@
       <c r="C43" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="12"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="17">
         <f>1302.1/60</f>
         <v>21.701666666666664</v>
@@ -1335,7 +1363,10 @@
       <c r="F43" s="18">
         <v>1302.0999999999999</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="19">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="H43" s="12">
         <v>129.19999999999999</v>
       </c>
     </row>
@@ -1343,7 +1374,7 @@
       <c r="C44" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="12"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="17">
         <f>979.5/60</f>
         <v>16.324999999999999</v>
@@ -1351,7 +1382,10 @@
       <c r="F44" s="12">
         <v>979.5</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="19">
+        <v>135</v>
+      </c>
+      <c r="H44" s="12">
         <v>135</v>
       </c>
     </row>
@@ -1360,6 +1394,7 @@
     <sortCondition ref="D36:D44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1370,6 +1405,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003259A36C4A547F44B955369E53BE8E3F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5acd7acae636e4acafb55b6a449d38ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2a75b999-46ea-40c0-9570-6b30446ff66a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ad1fee36f4b36fe5cc89a8efb12e836" ns3:_="">
     <xsd:import namespace="2a75b999-46ea-40c0-9570-6b30446ff66a"/>
@@ -1515,15 +1559,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB1F86DE-AB4C-4832-A7E0-AAE979277762}">
   <ds:schemaRefs>
@@ -1541,6 +1576,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC563DDF-B873-49CA-8554-8AE86FCAC509}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D65EC413-F0E8-4027-BFCD-25E2554F8075}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1556,12 +1599,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC563DDF-B873-49CA-8554-8AE86FCAC509}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>